<commit_message>
50% der tests fertig + bugfix
ein bug ist beim testen aufgetaucht, wo ein kunde nicht vorhanden war,
aber zum bedienen angekommen ist
</commit_message>
<xml_diff>
--- a/Stuffs/results.xlsx
+++ b/Stuffs/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>m</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>K4 avg wait</t>
+  </si>
+  <si>
+    <t>Avg max wait</t>
+  </si>
+  <si>
+    <t>Avg avg wait</t>
   </si>
 </sst>
 </file>
@@ -103,10 +109,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K121"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -399,11 +408,12 @@
     <col min="3" max="4" width="10.90625" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" customWidth="1"/>
     <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" customWidth="1"/>
-    <col min="8" max="10" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="11" width="10.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -423,22 +433,28 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,23 +473,31 @@
       <c r="F2" s="1">
         <v>8.0268999999999995</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
+        <f>AVERAGE(C2:F2)</f>
+        <v>14.284474999999997</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.72289999999999999</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>1.0851</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>1.1176999999999999</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>1.5215000000000001</v>
       </c>
-      <c r="K2">
+      <c r="L2" s="1">
+        <f>AVERAGE(H2:K2)</f>
+        <v>1.1118000000000001</v>
+      </c>
+      <c r="M2">
         <v>2926</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -492,23 +516,31 @@
       <c r="F3" s="1">
         <v>8.3247999999999998</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">AVERAGE(C3:F3)</f>
+        <v>9.1495999999999995</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.66180000000000005</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>1.3879999999999999</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1.4440999999999999</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>1.9659</v>
       </c>
-      <c r="K3">
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="1">AVERAGE(H3:K3)</f>
+        <v>1.3649499999999999</v>
+      </c>
+      <c r="M3">
         <v>2108</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -527,23 +559,31 @@
       <c r="F4" s="1">
         <v>12.9941</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>11.137274999999999</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.7722</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1.7367999999999999</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>2.0247999999999999</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>3.0823999999999998</v>
       </c>
-      <c r="K4">
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>1.9040499999999998</v>
+      </c>
+      <c r="M4">
         <v>1841</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -562,23 +602,31 @@
       <c r="F5" s="1">
         <v>8.6304999999999996</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>12.721325</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.87129999999999996</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>2.1444999999999999</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>2.7804000000000002</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>3.1095000000000002</v>
       </c>
-      <c r="K5">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>2.2264249999999999</v>
+      </c>
+      <c r="M5">
         <v>1740</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -597,23 +645,31 @@
       <c r="F6" s="1">
         <v>11.4948</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>11.211174999999999</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.99739999999999995</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>2.8144999999999998</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>3.1038000000000001</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>3.6360999999999999</v>
       </c>
-      <c r="K6">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>2.63795</v>
+      </c>
+      <c r="M6">
         <v>1701</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -632,23 +688,31 @@
       <c r="F7" s="1">
         <v>10.7141</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>11.918900000000001</v>
+      </c>
+      <c r="H7" s="1">
         <v>1.0682</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>3.0306000000000002</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>4.0849000000000002</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>5.13</v>
       </c>
-      <c r="K7">
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>3.3284250000000002</v>
+      </c>
+      <c r="M7">
         <v>1637</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -667,23 +731,31 @@
       <c r="F8" s="1">
         <v>9.2992000000000008</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>12.463550000000001</v>
+      </c>
+      <c r="H8" s="1">
         <v>1.1808000000000001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>3.8353999999999999</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>5.8034999999999997</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>4.5343</v>
       </c>
-      <c r="K8">
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>3.8384999999999998</v>
+      </c>
+      <c r="M8">
         <v>1609</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -702,23 +774,31 @@
       <c r="F9" s="1">
         <v>14.862500000000001</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>16.789175</v>
+      </c>
+      <c r="H9" s="1">
         <v>1.2445999999999999</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>4.8078000000000003</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>5.5476999999999999</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>8.0066000000000006</v>
       </c>
-      <c r="K9">
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>4.9016750000000009</v>
+      </c>
+      <c r="M9">
         <v>1589</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -737,23 +817,31 @@
       <c r="F10" s="1">
         <v>14.3611</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>17.346049999999998</v>
+      </c>
+      <c r="H10" s="1">
         <v>1.3986000000000001</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>6.0526</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>6.1733000000000002</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>7.4591000000000003</v>
       </c>
-      <c r="K10">
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>5.2709000000000001</v>
+      </c>
+      <c r="M10">
         <v>1589</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -772,33 +860,40 @@
       <c r="F11" s="1">
         <v>14.9086</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>16.384650000000001</v>
+      </c>
+      <c r="H11" s="1">
         <v>14.678000000000001</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>5.8958000000000004</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>7.7636000000000003</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>6.6784999999999997</v>
       </c>
-      <c r="K11">
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>8.7539750000000005</v>
+      </c>
+      <c r="M11">
         <v>1569</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -817,23 +912,31 @@
       <c r="F13" s="1">
         <v>7.6372999999999998</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>9.6738999999999997</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.7127</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>1.0096000000000001</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>1.0404</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>1.4468000000000001</v>
       </c>
-      <c r="K13">
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>1.0523750000000001</v>
+      </c>
+      <c r="M13">
         <v>2918</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -852,23 +955,31 @@
       <c r="F14" s="1">
         <v>11.551</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>8.8444000000000003</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.6552</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>1.3496999999999999</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>1.4629000000000001</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>2.0295999999999998</v>
       </c>
-      <c r="K14">
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>1.3743500000000002</v>
+      </c>
+      <c r="M14">
         <v>2129</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3</v>
       </c>
@@ -887,23 +998,31 @@
       <c r="F15" s="1">
         <v>7.1303999999999998</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>7.6153250000000003</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.83399999999999996</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>1.6539999999999999</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>1.8129999999999999</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>2.4293</v>
       </c>
-      <c r="K15">
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>1.6825749999999999</v>
+      </c>
+      <c r="M15">
         <v>1861</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4</v>
       </c>
@@ -922,23 +1041,31 @@
       <c r="F16" s="1">
         <v>8.7462999999999997</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>10.414724999999999</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.88970000000000005</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>2.1032000000000002</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>2.5672000000000001</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>3.1088</v>
       </c>
-      <c r="K16">
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>2.1672250000000002</v>
+      </c>
+      <c r="M16">
         <v>1738</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5</v>
       </c>
@@ -957,23 +1084,31 @@
       <c r="F17" s="1">
         <v>10.401</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>12.7316</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.95079999999999998</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>2.7482000000000002</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>3.3401000000000001</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>3.8471000000000002</v>
       </c>
-      <c r="K17">
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>2.7215500000000001</v>
+      </c>
+      <c r="M17">
         <v>1669</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>6</v>
       </c>
@@ -992,23 +1127,31 @@
       <c r="F18" s="1">
         <v>10.7141</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>11.918900000000001</v>
+      </c>
+      <c r="H18" s="1">
         <v>1.0682</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>3.0306000000000002</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>4.0849000000000002</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>5.13</v>
       </c>
-      <c r="K18">
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>3.3284250000000002</v>
+      </c>
+      <c r="M18">
         <v>1637</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1027,23 +1170,31 @@
       <c r="F19" s="1">
         <v>13.908200000000001</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>12.43215</v>
+      </c>
+      <c r="H19" s="1">
         <v>1.2250000000000001</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>4.0357000000000003</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>4.9584999999999999</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>6.4339000000000004</v>
       </c>
-      <c r="K19">
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>4.1632750000000005</v>
+      </c>
+      <c r="M19">
         <v>1625</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1062,23 +1213,31 @@
       <c r="F20" s="1">
         <v>11.334899999999999</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>13.715325</v>
+      </c>
+      <c r="H20" s="1">
         <v>1.2771999999999999</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>4.6963999999999997</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>5.0452000000000004</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>6.7752999999999997</v>
       </c>
-      <c r="K20">
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>4.4485250000000001</v>
+      </c>
+      <c r="M20">
         <v>1615</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1097,23 +1256,31 @@
       <c r="F21" s="1">
         <v>14.3611</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>17.346049999999998</v>
+      </c>
+      <c r="H21" s="1">
         <v>1.3986000000000001</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>6.0526</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>6.1733000000000002</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>7.4591000000000003</v>
       </c>
-      <c r="K21">
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>5.2709000000000001</v>
+      </c>
+      <c r="M21">
         <v>1589</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1132,743 +1299,2419 @@
       <c r="F22" s="1">
         <v>14.7559</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>16.893549999999998</v>
+      </c>
+      <c r="H22" s="1">
         <v>1.3976</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>6.1300999999999997</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>7.3781999999999996</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <v>8.8206000000000007</v>
       </c>
-      <c r="K22">
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>5.9316250000000004</v>
+      </c>
+      <c r="M22">
         <v>1559</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
+        <v>21.570699999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <v>11.005000000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6.8865999999999996</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10.5707</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>12.50825</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.73870000000000002</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1.0031000000000001</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.0085</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1.4976</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>1.0619750000000001</v>
+      </c>
+      <c r="M24">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <v>9.2531999999999996</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11.7766</v>
+      </c>
+      <c r="F25" s="1">
+        <v>8.0808999999999997</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>11.9116</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.68159999999999998</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1.3128</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1.5368999999999999</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2.3431000000000002</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>1.4685999999999999</v>
+      </c>
+      <c r="M25">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8.9795999999999996</v>
+      </c>
+      <c r="E26" s="1">
+        <v>8.6806000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>9.9146000000000001</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>11.527624999999999</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.78369999999999995</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1.6206</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1.8871</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>1.704725</v>
+      </c>
+      <c r="M26">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
+        <v>8.4695999999999998</v>
+      </c>
+      <c r="D27" s="1">
+        <v>11.674099999999999</v>
+      </c>
+      <c r="E27" s="1">
+        <v>10.929600000000001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>8.6442999999999994</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>9.9293999999999993</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2.0788000000000002</v>
+      </c>
+      <c r="J27" s="1">
+        <v>2.6042999999999998</v>
+      </c>
+      <c r="K27" s="1">
+        <v>3.2894000000000001</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="M27">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
+        <v>9.0907999999999998</v>
+      </c>
+      <c r="D28" s="1">
+        <v>11.900499999999999</v>
+      </c>
+      <c r="E28" s="1">
+        <v>11.1845</v>
+      </c>
+      <c r="F28" s="4">
+        <v>9.7969000000000008</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>10.493174999999999</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.98780000000000001</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2.7368000000000001</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3.2574000000000001</v>
+      </c>
+      <c r="K28" s="1">
+        <v>3.9483000000000001</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>2.7325750000000002</v>
+      </c>
+      <c r="M28">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>6</v>
       </c>
       <c r="B29">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
+        <v>8.4364000000000008</v>
+      </c>
+      <c r="D29" s="1">
+        <v>12.4171</v>
+      </c>
+      <c r="E29" s="1">
+        <v>11.3264</v>
+      </c>
+      <c r="F29" s="1">
+        <v>16.521100000000001</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>12.175250000000002</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3.0994000000000002</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.6116000000000001</v>
+      </c>
+      <c r="K29" s="1">
+        <v>5.1695000000000002</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>3.2396250000000002</v>
+      </c>
+      <c r="M29">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>7</v>
       </c>
       <c r="B30">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
+        <v>9.4323999999999995</v>
+      </c>
+      <c r="D30" s="1">
+        <v>15.191599999999999</v>
+      </c>
+      <c r="E30" s="1">
+        <v>13.9613</v>
+      </c>
+      <c r="F30" s="1">
+        <v>13.908200000000001</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>13.123374999999999</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1.2137</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4.1719999999999997</v>
+      </c>
+      <c r="J30" s="1">
+        <v>4.6063000000000001</v>
+      </c>
+      <c r="K30" s="1">
+        <v>6.0091999999999999</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>4.0003000000000002</v>
+      </c>
+      <c r="M30">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>8</v>
       </c>
       <c r="B31">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
+        <v>10.5413</v>
+      </c>
+      <c r="D31" s="1">
+        <v>18.134399999999999</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13.428599999999999</v>
+      </c>
+      <c r="F31" s="1">
+        <v>15.6881</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>14.448099999999998</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1.2554000000000001</v>
+      </c>
+      <c r="I31" s="1">
+        <v>4.8446999999999996</v>
+      </c>
+      <c r="J31" s="1">
+        <v>5.6435000000000004</v>
+      </c>
+      <c r="K31" s="1">
+        <v>7.0416999999999996</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>4.6963249999999999</v>
+      </c>
+      <c r="M31">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>9</v>
       </c>
       <c r="B32">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D32" s="1">
+        <v>18.435400000000001</v>
+      </c>
+      <c r="E32" s="1">
+        <v>12.839600000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>14.3611</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>16.042949999999998</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.39</v>
+      </c>
+      <c r="I32" s="1">
+        <v>5.7667000000000002</v>
+      </c>
+      <c r="J32" s="1">
+        <v>5.9885000000000002</v>
+      </c>
+      <c r="K32" s="1">
+        <v>8.0300999999999991</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>5.293825</v>
+      </c>
+      <c r="M32">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>10</v>
       </c>
       <c r="B33">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
+        <v>11.8279</v>
+      </c>
+      <c r="D33" s="1">
+        <v>20.902699999999999</v>
+      </c>
+      <c r="E33" s="1">
+        <v>20.087700000000002</v>
+      </c>
+      <c r="F33" s="1">
+        <v>14.7559</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>16.893549999999998</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.3976</v>
+      </c>
+      <c r="I33" s="1">
+        <v>6.1300999999999997</v>
+      </c>
+      <c r="J33" s="1">
+        <v>7.3781999999999996</v>
+      </c>
+      <c r="K33" s="1">
+        <v>8.8206000000000007</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>5.9316250000000004</v>
+      </c>
+      <c r="M33">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D35" s="1">
+        <v>10.1067</v>
+      </c>
+      <c r="E35" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>9.1935000000000002</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>11.983974999999999</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.74270000000000003</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1.0724</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1.5395000000000001</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>1.0973999999999999</v>
+      </c>
+      <c r="M35">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" s="1">
+        <v>9.6522000000000006</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.1039999999999992</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8.8674999999999997</v>
+      </c>
+      <c r="F36" s="1">
+        <v>8.0052000000000003</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>8.6572250000000004</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1.3839999999999999</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1.5174000000000001</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1.9495</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>1.3818999999999999</v>
+      </c>
+      <c r="M36">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>3</v>
       </c>
       <c r="B37">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" s="1">
+        <v>15.542199999999999</v>
+      </c>
+      <c r="D37" s="1">
+        <v>10.8111</v>
+      </c>
+      <c r="E37" s="1">
+        <v>12.215299999999999</v>
+      </c>
+      <c r="F37" s="1">
+        <v>9.6409000000000002</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>12.052375</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.8034</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1.5095000000000001</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1.8089999999999999</v>
+      </c>
+      <c r="K37" s="1">
+        <v>2.6366000000000001</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>1.6896249999999999</v>
+      </c>
+      <c r="M37">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>4</v>
       </c>
       <c r="B38">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D38" s="1">
+        <v>15.3186</v>
+      </c>
+      <c r="E38" s="1">
+        <v>11.691700000000001</v>
+      </c>
+      <c r="F38" s="1">
+        <v>11.6515</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>14.299374999999998</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.88160000000000005</v>
+      </c>
+      <c r="I38" s="1">
+        <v>2.1515</v>
+      </c>
+      <c r="J38" s="1">
+        <v>2.4340999999999999</v>
+      </c>
+      <c r="K38" s="1">
+        <v>3.7505999999999999</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>2.3044500000000001</v>
+      </c>
+      <c r="M38">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D39" s="1">
+        <v>12.679</v>
+      </c>
+      <c r="E39" s="1">
+        <v>11.1005</v>
+      </c>
+      <c r="F39" s="1">
+        <v>11.5084</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>13.455900000000002</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2.5554999999999999</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3.3328000000000002</v>
+      </c>
+      <c r="K39" s="1">
+        <v>5.7343999999999999</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>3.1369249999999997</v>
+      </c>
+      <c r="M39">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>6</v>
       </c>
       <c r="B40">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" s="1">
+        <v>8.3137000000000008</v>
+      </c>
+      <c r="D40" s="1">
+        <v>12.411099999999999</v>
+      </c>
+      <c r="E40" s="1">
+        <v>13.1347</v>
+      </c>
+      <c r="F40" s="1">
+        <v>9.7591999999999999</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>10.904675000000001</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1.0206</v>
+      </c>
+      <c r="I40" s="1">
+        <v>3.2393000000000001</v>
+      </c>
+      <c r="J40" s="1">
+        <v>3.6215000000000002</v>
+      </c>
+      <c r="K40" s="1">
+        <v>5.4782000000000002</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>3.3399000000000001</v>
+      </c>
+      <c r="M40">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>7</v>
       </c>
       <c r="B41">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" s="1">
+        <v>9.4695999999999998</v>
+      </c>
+      <c r="D41" s="1">
+        <v>14.632899999999999</v>
+      </c>
+      <c r="E41" s="1">
+        <v>11.5524</v>
+      </c>
+      <c r="F41" s="1">
+        <v>13.065099999999999</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>12.18</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1.1317999999999999</v>
+      </c>
+      <c r="I41" s="1">
+        <v>3.6480999999999999</v>
+      </c>
+      <c r="J41" s="1">
+        <v>4.2287999999999997</v>
+      </c>
+      <c r="K41" s="1">
+        <v>6.1318999999999999</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>3.7851499999999998</v>
+      </c>
+      <c r="M41">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>8</v>
       </c>
       <c r="B42">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D42" s="1">
+        <v>17.346</v>
+      </c>
+      <c r="E42" s="1">
+        <v>17.0793</v>
+      </c>
+      <c r="F42" s="1">
+        <v>13.9709</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>16.732975</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1.2586999999999999</v>
+      </c>
+      <c r="I42" s="1">
+        <v>4.7073</v>
+      </c>
+      <c r="J42" s="1">
+        <v>5.0362999999999998</v>
+      </c>
+      <c r="K42" s="1">
+        <v>7.2328999999999999</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>4.5587999999999997</v>
+      </c>
+      <c r="M42">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>9</v>
       </c>
       <c r="B43">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D43" s="1">
+        <v>20.000399999999999</v>
+      </c>
+      <c r="E43" s="1">
+        <v>14.0585</v>
+      </c>
+      <c r="F43" s="1">
+        <v>14.945</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>16.884900000000002</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1.4365000000000001</v>
+      </c>
+      <c r="I43" s="1">
+        <v>5.8141999999999996</v>
+      </c>
+      <c r="J43" s="1">
+        <v>5.7123999999999997</v>
+      </c>
+      <c r="K43" s="1">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>5.1537750000000004</v>
+      </c>
+      <c r="M43">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>10</v>
       </c>
       <c r="B44">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>22.086300000000001</v>
+      </c>
+      <c r="E44" s="1">
+        <v>19.394400000000001</v>
+      </c>
+      <c r="F44" s="1">
+        <v>16.382100000000001</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>19.099625000000003</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1.4529000000000001</v>
+      </c>
+      <c r="I44" s="1">
+        <v>6.4394999999999998</v>
+      </c>
+      <c r="J44" s="1">
+        <v>7.9283999999999999</v>
+      </c>
+      <c r="K44" s="1">
+        <v>6.9241000000000001</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>5.6862250000000003</v>
+      </c>
+      <c r="M44">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D46" s="1">
+        <v>7.5523999999999996</v>
+      </c>
+      <c r="E46" s="1">
+        <v>7.3833000000000002</v>
+      </c>
+      <c r="F46" s="1">
+        <v>8.1327999999999996</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>10.401049999999998</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0.76229999999999998</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0.95350000000000001</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0.92410000000000003</v>
+      </c>
+      <c r="K46" s="5">
+        <v>1.2875000000000001</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>0.98185</v>
+      </c>
+      <c r="M46">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" s="1">
+        <v>7.3308</v>
+      </c>
+      <c r="D47" s="1">
+        <v>8.4695999999999998</v>
+      </c>
+      <c r="E47" s="1">
+        <v>8.4140999999999995</v>
+      </c>
+      <c r="F47" s="1">
+        <v>7.6210000000000004</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>7.9588750000000008</v>
+      </c>
+      <c r="H47" s="5">
+        <v>0.62309999999999999</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1.2498</v>
+      </c>
+      <c r="J47" s="5">
+        <v>1.3996999999999999</v>
+      </c>
+      <c r="K47" s="5">
+        <v>1.7283999999999999</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>1.2502499999999999</v>
+      </c>
+      <c r="M47">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D48" s="1">
+        <v>14.2813</v>
+      </c>
+      <c r="E48" s="1">
+        <v>8.5599000000000007</v>
+      </c>
+      <c r="F48" s="1">
+        <v>10.679600000000001</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>13.014125</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0.77939999999999998</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1.6408</v>
+      </c>
+      <c r="J48" s="5">
+        <v>2.0068000000000001</v>
+      </c>
+      <c r="K48" s="5">
+        <v>2.7414000000000001</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="1"/>
+        <v>1.7921</v>
+      </c>
+      <c r="M48">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
+        <v>9.6522000000000006</v>
+      </c>
+      <c r="D49" s="1">
+        <v>17.092199999999998</v>
+      </c>
+      <c r="E49" s="1">
+        <v>9.9643999999999995</v>
+      </c>
+      <c r="F49" s="1">
+        <v>13.1821</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>12.472724999999999</v>
+      </c>
+      <c r="H49" s="5">
+        <v>0.86950000000000005</v>
+      </c>
+      <c r="I49" s="5">
+        <v>2.0981999999999998</v>
+      </c>
+      <c r="J49" s="5">
+        <v>2.6941000000000002</v>
+      </c>
+      <c r="K49" s="5">
+        <v>3.8538999999999999</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="1"/>
+        <v>2.3789249999999997</v>
+      </c>
+      <c r="M49">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>5</v>
       </c>
       <c r="B50">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" s="1">
+        <v>8.9514999999999993</v>
+      </c>
+      <c r="D50" s="1">
+        <v>11.6639</v>
+      </c>
+      <c r="E50" s="1">
+        <v>10.392799999999999</v>
+      </c>
+      <c r="F50" s="1">
+        <v>8.4307999999999996</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>9.85975</v>
+      </c>
+      <c r="H50" s="5">
+        <v>0.98529999999999995</v>
+      </c>
+      <c r="I50" s="5">
+        <v>2.4779</v>
+      </c>
+      <c r="J50" s="5">
+        <v>2.9948000000000001</v>
+      </c>
+      <c r="K50" s="5">
+        <v>3.1979000000000002</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="1"/>
+        <v>2.4139750000000002</v>
+      </c>
+      <c r="M50">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
       <c r="B51">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51" s="1">
+        <v>8.8779000000000003</v>
+      </c>
+      <c r="D51" s="1">
+        <v>13.8116</v>
+      </c>
+      <c r="E51" s="1">
+        <v>12.5198</v>
+      </c>
+      <c r="F51" s="1">
+        <v>11.0564</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>11.566424999999999</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1.0576000000000001</v>
+      </c>
+      <c r="I51" s="5">
+        <v>3.3864000000000001</v>
+      </c>
+      <c r="J51" s="5">
+        <v>3.6164000000000001</v>
+      </c>
+      <c r="K51" s="5">
+        <v>4.8681000000000001</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="1"/>
+        <v>3.2321249999999999</v>
+      </c>
+      <c r="M51">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>7</v>
       </c>
       <c r="B52">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" s="1">
+        <v>10.430400000000001</v>
+      </c>
+      <c r="D52" s="1">
+        <v>14.228400000000001</v>
+      </c>
+      <c r="E52" s="1">
+        <v>13.526899999999999</v>
+      </c>
+      <c r="F52" s="1">
+        <v>12.7903</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>12.744</v>
+      </c>
+      <c r="H52" s="5">
+        <v>1.1689000000000001</v>
+      </c>
+      <c r="I52" s="5">
+        <v>3.8349000000000002</v>
+      </c>
+      <c r="J52" s="5">
+        <v>5.3361999999999998</v>
+      </c>
+      <c r="K52" s="5">
+        <v>7.2793000000000001</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>4.4048249999999998</v>
+      </c>
+      <c r="M52">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>8</v>
       </c>
       <c r="B53">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D53" s="1">
+        <v>17.346</v>
+      </c>
+      <c r="E53" s="1">
+        <v>14.5631</v>
+      </c>
+      <c r="F53" s="1">
+        <v>11.432499999999999</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>15.469324999999998</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="I53" s="5">
+        <v>4.7328999999999999</v>
+      </c>
+      <c r="J53" s="5">
+        <v>5.0395000000000003</v>
+      </c>
+      <c r="K53" s="5">
+        <v>6.0491000000000001</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="1"/>
+        <v>4.2571750000000002</v>
+      </c>
+      <c r="M53">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9</v>
       </c>
       <c r="B54">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D54" s="1">
+        <v>19.724799999999998</v>
+      </c>
+      <c r="E54" s="1">
+        <v>15.7743</v>
+      </c>
+      <c r="F54" s="1">
+        <v>14.144299999999999</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>17.044774999999998</v>
+      </c>
+      <c r="H54" s="5">
+        <v>1.4217</v>
+      </c>
+      <c r="I54" s="5">
+        <v>5.4256000000000002</v>
+      </c>
+      <c r="J54" s="5">
+        <v>5.4012000000000002</v>
+      </c>
+      <c r="K54" s="5">
+        <v>8.2078000000000007</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="1"/>
+        <v>5.1140749999999997</v>
+      </c>
+      <c r="M54">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>10</v>
       </c>
       <c r="B55">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55" s="3">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D55" s="3">
+        <v>22.959399999999999</v>
+      </c>
+      <c r="E55" s="3">
+        <v>18.3856</v>
+      </c>
+      <c r="F55" s="3">
+        <v>19.499700000000001</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>19.845099999999999</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1.4520999999999999</v>
+      </c>
+      <c r="I55" s="5">
+        <v>5.9851000000000001</v>
+      </c>
+      <c r="J55" s="5">
+        <v>6.8487</v>
+      </c>
+      <c r="K55" s="5">
+        <v>10.5063</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>6.1980500000000003</v>
+      </c>
+      <c r="M55">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
       <c r="B57">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" s="1">
+        <v>21.570699999999999</v>
+      </c>
+      <c r="D57" s="1">
+        <v>10.3649</v>
+      </c>
+      <c r="E57" s="1">
+        <v>11.127000000000001</v>
+      </c>
+      <c r="F57" s="1">
+        <v>8.6533999999999995</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>12.929</v>
+      </c>
+      <c r="H57" s="5">
+        <v>0.79379999999999995</v>
+      </c>
+      <c r="I57" s="5">
+        <v>0.9708</v>
+      </c>
+      <c r="J57" s="5">
+        <v>1.0548</v>
+      </c>
+      <c r="K57" s="5">
+        <v>1.4964999999999999</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="1"/>
+        <v>1.078975</v>
+      </c>
+      <c r="M57">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
       <c r="B58">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58" s="1">
+        <v>16.206900000000001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>12.913600000000001</v>
+      </c>
+      <c r="E58" s="1">
+        <v>12.0877</v>
+      </c>
+      <c r="F58" s="1">
+        <v>9.4550999999999998</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>12.665825</v>
+      </c>
+      <c r="H58" s="5">
+        <v>0.65610000000000002</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1.3132999999999999</v>
+      </c>
+      <c r="J58" s="5">
+        <v>1.4912000000000001</v>
+      </c>
+      <c r="K58" s="5">
+        <v>2.2124000000000001</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="1"/>
+        <v>1.41825</v>
+      </c>
+      <c r="M58">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>3</v>
       </c>
       <c r="B59">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59" s="1">
+        <v>9.6522000000000006</v>
+      </c>
+      <c r="D59" s="1">
+        <v>9.1736000000000004</v>
+      </c>
+      <c r="E59" s="1">
+        <v>12.167</v>
+      </c>
+      <c r="F59" s="1">
+        <v>10.850199999999999</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>10.460750000000001</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0.76129999999999998</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1.6226</v>
+      </c>
+      <c r="J59" s="5">
+        <v>1.9073</v>
+      </c>
+      <c r="K59" s="5">
+        <v>2.5592999999999999</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="1"/>
+        <v>1.7126250000000001</v>
+      </c>
+      <c r="M59">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>4</v>
       </c>
       <c r="B60">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60" s="1">
+        <v>15.542199999999999</v>
+      </c>
+      <c r="D60" s="1">
+        <v>11.170400000000001</v>
+      </c>
+      <c r="E60" s="1">
+        <v>11.5791</v>
+      </c>
+      <c r="F60" s="1">
+        <v>7.7732999999999999</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>11.516250000000001</v>
+      </c>
+      <c r="H60" s="5">
+        <v>0.85219999999999996</v>
+      </c>
+      <c r="I60" s="5">
+        <v>2.0268000000000002</v>
+      </c>
+      <c r="J60" s="5">
+        <v>2.4592999999999998</v>
+      </c>
+      <c r="K60" s="5">
+        <v>2.9167999999999998</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="1"/>
+        <v>2.0637750000000001</v>
+      </c>
+      <c r="M60">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>5</v>
       </c>
       <c r="B61">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61" s="1">
+        <v>18.535699999999999</v>
+      </c>
+      <c r="D61" s="1">
+        <v>14.565899999999999</v>
+      </c>
+      <c r="E61" s="1">
+        <v>11.8574</v>
+      </c>
+      <c r="F61" s="1">
+        <v>15.3741</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>15.083274999999999</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1.0439000000000001</v>
+      </c>
+      <c r="I61" s="5">
+        <v>2.5272000000000001</v>
+      </c>
+      <c r="J61" s="5">
+        <v>3.4935</v>
+      </c>
+      <c r="K61" s="5">
+        <v>5.3327999999999998</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="1"/>
+        <v>3.0993500000000003</v>
+      </c>
+      <c r="M61">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>6</v>
       </c>
       <c r="B62">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G62" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L62" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>7</v>
       </c>
       <c r="B63">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L63" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
       <c r="B64">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G64" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L64" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>9</v>
       </c>
       <c r="B65">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G65" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L65" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>10</v>
       </c>
       <c r="B66">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L66" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1</v>
       </c>
       <c r="B68">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G68" t="e">
+        <f t="shared" ref="G67:G121" si="2">AVERAGE(C68:F68)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L68" t="e">
+        <f t="shared" ref="L67:L121" si="3">AVERAGE(H68:K68)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>2</v>
       </c>
       <c r="B69">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G69" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L69" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>3</v>
       </c>
       <c r="B70">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G70" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L70" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>4</v>
       </c>
       <c r="B71">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G71" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L71" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>5</v>
       </c>
       <c r="B72">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G72" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L72" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>6</v>
       </c>
       <c r="B73">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G73" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L73" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>7</v>
       </c>
       <c r="B74">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L74" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>8</v>
       </c>
       <c r="B75">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G75" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L75" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>9</v>
       </c>
       <c r="B76">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G76" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L76" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
       <c r="B77">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G77" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L77" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1</v>
       </c>
       <c r="B79">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G79" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L79" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2</v>
       </c>
       <c r="B80">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G80" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L80" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
       <c r="B81">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G81" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L81" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>4</v>
       </c>
       <c r="B82">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G82" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L82" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>5</v>
       </c>
       <c r="B83">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G83" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L83" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>6</v>
       </c>
       <c r="B84">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G84" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L84" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>7</v>
       </c>
       <c r="B85">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G85" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L85" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>8</v>
       </c>
       <c r="B86">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G86" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L86" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>9</v>
       </c>
       <c r="B87">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G87" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L87" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>10</v>
       </c>
       <c r="B88">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G88" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L88" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1</v>
       </c>
       <c r="B90">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G90" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L90" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2</v>
       </c>
       <c r="B91">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G91" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L91" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>3</v>
       </c>
       <c r="B92">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G92" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L92" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>4</v>
       </c>
       <c r="B93">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G93" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L93" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>5</v>
       </c>
       <c r="B94">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G94" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L94" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>6</v>
       </c>
       <c r="B95">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G95" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L95" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>7</v>
       </c>
       <c r="B96">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L96" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>8</v>
       </c>
       <c r="B97">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G97" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L97" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>9</v>
       </c>
       <c r="B98">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G98" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L98" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>10</v>
       </c>
       <c r="B99">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G99" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L99" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1</v>
       </c>
       <c r="B101">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G101" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L101" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2</v>
       </c>
       <c r="B102">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G102" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L102" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>3</v>
       </c>
       <c r="B103">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G103" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L103" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>4</v>
       </c>
       <c r="B104">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G104" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L104" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>5</v>
       </c>
       <c r="B105">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G105" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L105" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>6</v>
       </c>
       <c r="B106">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G106" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L106" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>7</v>
       </c>
       <c r="B107">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G107" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L107" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>8</v>
       </c>
       <c r="B108">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G108" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L108" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>9</v>
       </c>
       <c r="B109">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G109" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L109" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>10</v>
       </c>
       <c r="B110">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G110" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L110" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G112" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L112" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2</v>
       </c>
       <c r="B113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G113" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L113" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>3</v>
       </c>
       <c r="B114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G114" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L114" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>4</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G115" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L115" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>5</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G116" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L116" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>6</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G117" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L117" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>7</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G118" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L118" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>8</v>
       </c>
       <c r="B119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G119" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L119" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>9</v>
       </c>
       <c r="B120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G120" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L120" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>10</v>
       </c>
       <c r="B121">
         <v>1</v>
       </c>
+      <c r="G121" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L121" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2:G121" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>